<commit_message>
finished now, i hope
</commit_message>
<xml_diff>
--- a/kostnadder.xlsx
+++ b/kostnadder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\G-Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F6903A3-5F8D-4AA9-B3B5-07EECE612F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7942D6-73BC-4FE1-BC8E-41D69A346E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3030" yWindow="1260" windowWidth="21600" windowHeight="11385" xr2:uid="{C7033952-0C0C-4786-B4E8-A82CA507607F}"/>
+    <workbookView xWindow="3030" yWindow="1275" windowWidth="21600" windowHeight="11370" xr2:uid="{C7033952-0C0C-4786-B4E8-A82CA507607F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>domene</t>
   </si>
   <si>
-    <t>arbeid på protorypen</t>
-  </si>
-  <si>
     <t>arbeid for og ferdigstille</t>
   </si>
   <si>
@@ -51,6 +48,12 @@
   </si>
   <si>
     <t>SUM</t>
+  </si>
+  <si>
+    <t>lisenser</t>
+  </si>
+  <si>
+    <t>arbeid for prototype</t>
   </si>
 </sst>
 </file>
@@ -422,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2380B7C2-02F5-4292-92A8-92F5CD5E12DB}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -435,7 +438,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -448,27 +451,35 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B3">
-        <v>2000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B4">
-        <v>1000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B5">
-        <f>SUM(B2:B4)</f>
-        <v>3150</v>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <f>SUM(B2:B5)</f>
+        <v>5650</v>
       </c>
     </row>
   </sheetData>

</xml_diff>